<commit_message>
Add more stats for every subset
</commit_message>
<xml_diff>
--- a/kaggle3/list_categories_dataset_draft.xlsx
+++ b/kaggle3/list_categories_dataset_draft.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="130">
   <si>
     <t xml:space="preserve">Total number of sounds in final dataset</t>
   </si>
@@ -34,15 +34,24 @@
     <t xml:space="preserve">num dev HQ</t>
   </si>
   <si>
-    <t xml:space="preserve">num dev LQ</t>
+    <t xml:space="preserve">num dev LQ (initially)</t>
   </si>
   <si>
     <t xml:space="preserve">num dev final</t>
   </si>
   <si>
+    <t xml:space="preserve">of which dev LQ is:</t>
+  </si>
+  <si>
     <t xml:space="preserve">num eval</t>
   </si>
   <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manual verified examples in each category</t>
+  </si>
+  <si>
     <t xml:space="preserve">num dev LQ prior</t>
   </si>
   <si>
@@ -334,40 +343,73 @@
     <t xml:space="preserve">/m/02yds9</t>
   </si>
   <si>
-    <t xml:space="preserve">total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total HQ</t>
+    <t xml:space="preserve">total check</t>
   </si>
   <si>
     <t xml:space="preserve">min</t>
   </si>
   <si>
-    <t xml:space="preserve">in per respect to all data</t>
-  </si>
-  <si>
     <t xml:space="preserve">max</t>
   </si>
   <si>
     <t xml:space="preserve">median</t>
   </si>
   <si>
+    <t xml:space="preserve">total HQ in the dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">categories in grey: most of them, 33</t>
   </si>
   <si>
+    <t xml:space="preserve">in percentage respect to WHOLE dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">leveraging large subsets of data with less reliable annotations, and bootstrapping these using a smaller subset with reliable annotations</t>
   </si>
   <si>
+    <t xml:space="preserve">total LQ in the dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 categories in green:</t>
   </si>
   <si>
+    <t xml:space="preserve">sum</t>
+  </si>
+  <si>
     <t xml:space="preserve">leveraging a comparable amount of HQ and LQ annotations</t>
   </si>
   <si>
     <t xml:space="preserve">5 remaining categories</t>
   </si>
   <si>
+    <t xml:space="preserve">eval set with respect to WHOLE dataset</t>
+  </si>
+  <si>
     <t xml:space="preserve">mostly HQ: only a few LQ (that should be removed for clarity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ portion in dev w resp to WHOLE dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all LQ in WHOLE dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this numbers are subject to minor changes due to failures in the final conversion to PCM 16 bit 44.100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev set with respecto to WHOLE dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">summed with eval set with respect to whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ portion within the dev set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQ portion within dev set</t>
   </si>
 </sst>
 </file>
@@ -409,7 +451,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,8 +472,44 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6666"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC66FF"/>
+        <bgColor rgb="FF9999FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9900FF"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF66"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor rgb="FF99FFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -469,7 +547,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -486,7 +564,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,7 +628,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -513,16 +639,16 @@
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF9900FF"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6666"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -537,9 +663,9 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF66"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF66FFFF"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFCC66FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33FF99"/>
@@ -567,22 +693,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I54" activeCellId="0" sqref="I54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="45.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,16 +741,25 @@
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>38</v>
@@ -629,26 +767,34 @@
       <c r="D3" s="2" t="n">
         <v>621</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="0" t="n">
         <v>272</v>
       </c>
       <c r="F3" s="0" t="n">
+        <f aca="false">E3-C3</f>
+        <v>234</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">SUM(E3:F3)</f>
+      <c r="H3" s="0" t="n">
+        <f aca="false">SUM(E3,G3)</f>
         <v>287</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="J3" s="0" t="n">
+        <f aca="false">C3+G3</f>
+        <v>53</v>
+      </c>
+      <c r="O3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>29</v>
@@ -656,26 +802,34 @@
       <c r="D4" s="2" t="n">
         <v>278</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="0" t="n">
         <v>282</v>
       </c>
       <c r="F4" s="0" t="n">
+        <f aca="false">E4-C4</f>
+        <v>253</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">SUM(E4:F4)</f>
+      <c r="H4" s="0" t="n">
+        <f aca="false">SUM(E4,G4)</f>
         <v>296</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="J4" s="0" t="n">
+        <f aca="false">C4+G4</f>
+        <v>43</v>
+      </c>
+      <c r="O4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>55</v>
@@ -683,26 +837,34 @@
       <c r="D5" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="0" t="n">
         <v>113</v>
       </c>
       <c r="F5" s="0" t="n">
+        <f aca="false">E5-C5</f>
+        <v>58</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">SUM(E5:F5)</f>
+      <c r="H5" s="0" t="n">
+        <f aca="false">SUM(E5,G5)</f>
         <v>137</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="J5" s="0" t="n">
+        <f aca="false">C5+G5</f>
+        <v>79</v>
+      </c>
+      <c r="O5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>39</v>
@@ -710,26 +872,34 @@
       <c r="D6" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="0" t="n">
         <v>94</v>
       </c>
       <c r="F6" s="0" t="n">
+        <f aca="false">E6-C6</f>
+        <v>55</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <f aca="false">SUM(E6:F6)</f>
+      <c r="H6" s="0" t="n">
+        <f aca="false">SUM(E6,G6)</f>
         <v>111</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="J6" s="0" t="n">
+        <f aca="false">C6+G6</f>
+        <v>56</v>
+      </c>
+      <c r="O6" s="0" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>61</v>
@@ -737,26 +907,34 @@
       <c r="D7" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <v>264</v>
       </c>
       <c r="F7" s="0" t="n">
+        <f aca="false">E7-C7</f>
+        <v>203</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <f aca="false">SUM(E7:F7)</f>
+      <c r="H7" s="0" t="n">
+        <f aca="false">SUM(E7,G7)</f>
         <v>291</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="J7" s="0" t="n">
+        <f aca="false">C7+G7</f>
+        <v>88</v>
+      </c>
+      <c r="O7" s="0" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>53</v>
@@ -764,26 +942,34 @@
       <c r="D8" s="2" t="n">
         <v>408</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>292</v>
       </c>
       <c r="F8" s="0" t="n">
+        <f aca="false">E8-C8</f>
+        <v>239</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">SUM(E8:F8)</f>
+      <c r="H8" s="0" t="n">
+        <f aca="false">SUM(E8,G8)</f>
         <v>314</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="J8" s="0" t="n">
+        <f aca="false">C8+G8</f>
+        <v>75</v>
+      </c>
+      <c r="O8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>36</v>
@@ -791,26 +977,34 @@
       <c r="D9" s="3" t="n">
         <v>62</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="0" t="n">
         <v>98</v>
       </c>
       <c r="F9" s="0" t="n">
+        <f aca="false">E9-C9</f>
+        <v>62</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">SUM(E9:F9)</f>
+      <c r="H9" s="0" t="n">
+        <f aca="false">SUM(E9,G9)</f>
         <v>113</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="J9" s="0" t="n">
+        <f aca="false">C9+G9</f>
+        <v>51</v>
+      </c>
+      <c r="O9" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>46</v>
@@ -818,26 +1012,34 @@
       <c r="D10" s="2" t="n">
         <v>552</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <v>298</v>
       </c>
       <c r="F10" s="0" t="n">
+        <f aca="false">E10-C10</f>
+        <v>252</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">SUM(E10:F10)</f>
+      <c r="H10" s="0" t="n">
+        <f aca="false">SUM(E10,G10)</f>
         <v>318</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="J10" s="0" t="n">
+        <f aca="false">C10+G10</f>
+        <v>66</v>
+      </c>
+      <c r="O10" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>157</v>
@@ -849,22 +1051,30 @@
         <v>159</v>
       </c>
       <c r="F11" s="0" t="n">
+        <f aca="false">E11-C11</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">SUM(E11:F11)</f>
+      <c r="H11" s="0" t="n">
+        <f aca="false">SUM(E11,G11)</f>
         <v>226</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="J11" s="0" t="n">
+        <f aca="false">C11+G11</f>
+        <v>224</v>
+      </c>
+      <c r="O11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>63</v>
@@ -876,22 +1086,30 @@
         <v>295</v>
       </c>
       <c r="F12" s="0" t="n">
+        <f aca="false">E12-C12</f>
+        <v>232</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">SUM(E12:F12)</f>
+      <c r="H12" s="0" t="n">
+        <f aca="false">SUM(E12,G12)</f>
         <v>323</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="J12" s="0" t="n">
+        <f aca="false">C12+G12</f>
+        <v>91</v>
+      </c>
+      <c r="O12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>37</v>
@@ -903,22 +1121,30 @@
         <v>161</v>
       </c>
       <c r="F13" s="0" t="n">
+        <f aca="false">E13-C13</f>
+        <v>124</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">SUM(E13:F13)</f>
+      <c r="H13" s="0" t="n">
+        <f aca="false">SUM(E13,G13)</f>
         <v>177</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="J13" s="0" t="n">
+        <f aca="false">C13+G13</f>
+        <v>53</v>
+      </c>
+      <c r="O13" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>36</v>
@@ -930,22 +1156,30 @@
         <v>122</v>
       </c>
       <c r="F14" s="0" t="n">
+        <f aca="false">E14-C14</f>
+        <v>86</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">SUM(E14:F14)</f>
+      <c r="H14" s="0" t="n">
+        <f aca="false">SUM(E14,G14)</f>
         <v>138</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="J14" s="0" t="n">
+        <f aca="false">C14+G14</f>
+        <v>52</v>
+      </c>
+      <c r="O14" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>54</v>
@@ -957,22 +1191,30 @@
         <v>204</v>
       </c>
       <c r="F15" s="0" t="n">
+        <f aca="false">E15-C15</f>
+        <v>150</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">SUM(E15:F15)</f>
+      <c r="H15" s="0" t="n">
+        <f aca="false">SUM(E15,G15)</f>
         <v>226</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="J15" s="0" t="n">
+        <f aca="false">C15+G15</f>
+        <v>76</v>
+      </c>
+      <c r="O15" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>39</v>
@@ -984,22 +1226,30 @@
         <v>290</v>
       </c>
       <c r="F16" s="0" t="n">
+        <f aca="false">E16-C16</f>
+        <v>251</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">SUM(E16:F16)</f>
+      <c r="H16" s="0" t="n">
+        <f aca="false">SUM(E16,G16)</f>
         <v>306</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="J16" s="0" t="n">
+        <f aca="false">C16+G16</f>
+        <v>55</v>
+      </c>
+      <c r="O16" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>103</v>
@@ -1011,22 +1261,30 @@
         <v>104</v>
       </c>
       <c r="F17" s="0" t="n">
+        <f aca="false">E17-C17</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">SUM(E17:F17)</f>
+      <c r="H17" s="0" t="n">
+        <f aca="false">SUM(E17,G17)</f>
         <v>147</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="J17" s="0" t="n">
+        <f aca="false">C17+G17</f>
+        <v>146</v>
+      </c>
+      <c r="O17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>135</v>
@@ -1038,22 +1296,30 @@
         <v>144</v>
       </c>
       <c r="F18" s="0" t="n">
+        <f aca="false">E18-C18</f>
+        <v>9</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">SUM(E18:F18)</f>
+      <c r="H18" s="0" t="n">
+        <f aca="false">SUM(E18,G18)</f>
         <v>202</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="J18" s="0" t="n">
+        <f aca="false">C18+G18</f>
+        <v>193</v>
+      </c>
+      <c r="O18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>37</v>
@@ -1065,22 +1331,30 @@
         <v>293</v>
       </c>
       <c r="F19" s="0" t="n">
+        <f aca="false">E19-C19</f>
+        <v>256</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">SUM(E19:F19)</f>
+      <c r="H19" s="0" t="n">
+        <f aca="false">SUM(E19,G19)</f>
         <v>309</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="J19" s="0" t="n">
+        <f aca="false">C19+G19</f>
+        <v>53</v>
+      </c>
+      <c r="O19" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>95</v>
@@ -1092,22 +1366,30 @@
         <v>195</v>
       </c>
       <c r="F20" s="0" t="n">
+        <f aca="false">E20-C20</f>
+        <v>100</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">SUM(E20:F20)</f>
+      <c r="H20" s="0" t="n">
+        <f aca="false">SUM(E20,G20)</f>
         <v>236</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="J20" s="0" t="n">
+        <f aca="false">C20+G20</f>
+        <v>136</v>
+      </c>
+      <c r="O20" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>99</v>
@@ -1119,22 +1401,30 @@
         <v>300</v>
       </c>
       <c r="F21" s="0" t="n">
+        <f aca="false">E21-C21</f>
+        <v>201</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">SUM(E21:F21)</f>
+      <c r="H21" s="0" t="n">
+        <f aca="false">SUM(E21,G21)</f>
         <v>342</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="J21" s="0" t="n">
+        <f aca="false">C21+G21</f>
+        <v>141</v>
+      </c>
+      <c r="O21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>148</v>
@@ -1146,22 +1436,30 @@
         <v>295</v>
       </c>
       <c r="F22" s="0" t="n">
+        <f aca="false">E22-C22</f>
+        <v>147</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">SUM(E22:F22)</f>
+      <c r="H22" s="0" t="n">
+        <f aca="false">SUM(E22,G22)</f>
         <v>359</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="J22" s="0" t="n">
+        <f aca="false">C22+G22</f>
+        <v>212</v>
+      </c>
+      <c r="O22" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>133</v>
@@ -1173,22 +1471,30 @@
         <v>296</v>
       </c>
       <c r="F23" s="0" t="n">
+        <f aca="false">E23-C23</f>
+        <v>163</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">SUM(E23:F23)</f>
+      <c r="H23" s="0" t="n">
+        <f aca="false">SUM(E23,G23)</f>
         <v>353</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="J23" s="0" t="n">
+        <f aca="false">C23+G23</f>
+        <v>190</v>
+      </c>
+      <c r="O23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>134</v>
@@ -1200,22 +1506,30 @@
         <v>134</v>
       </c>
       <c r="F24" s="0" t="n">
+        <f aca="false">E24-C24</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">SUM(E24:F24)</f>
+      <c r="H24" s="0" t="n">
+        <f aca="false">SUM(E24,G24)</f>
         <v>192</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="J24" s="0" t="n">
+        <f aca="false">C24+G24</f>
+        <v>192</v>
+      </c>
+      <c r="O24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>32</v>
@@ -1227,22 +1541,30 @@
         <v>292</v>
       </c>
       <c r="F25" s="0" t="n">
+        <f aca="false">E25-C25</f>
+        <v>260</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">SUM(E25:F25)</f>
+      <c r="H25" s="0" t="n">
+        <f aca="false">SUM(E25,G25)</f>
         <v>306</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="J25" s="0" t="n">
+        <f aca="false">C25+G25</f>
+        <v>46</v>
+      </c>
+      <c r="O25" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>131</v>
@@ -1254,22 +1576,30 @@
         <v>294</v>
       </c>
       <c r="F26" s="0" t="n">
+        <f aca="false">E26-C26</f>
+        <v>163</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">SUM(E26:F26)</f>
+      <c r="H26" s="0" t="n">
+        <f aca="false">SUM(E26,G26)</f>
         <v>353</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="J26" s="0" t="n">
+        <f aca="false">C26+G26</f>
+        <v>190</v>
+      </c>
+      <c r="O26" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>94</v>
@@ -1281,22 +1611,30 @@
         <v>241</v>
       </c>
       <c r="F27" s="0" t="n">
+        <f aca="false">E27-C27</f>
+        <v>147</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">SUM(E27:F27)</f>
+      <c r="H27" s="0" t="n">
+        <f aca="false">SUM(E27,G27)</f>
         <v>282</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="J27" s="0" t="n">
+        <f aca="false">C27+G27</f>
+        <v>135</v>
+      </c>
+      <c r="O27" s="0" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>62</v>
@@ -1308,22 +1646,30 @@
         <v>112</v>
       </c>
       <c r="F28" s="0" t="n">
+        <f aca="false">E28-C28</f>
+        <v>50</v>
+      </c>
+      <c r="G28" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">SUM(E28:F28)</f>
+      <c r="H28" s="0" t="n">
+        <f aca="false">SUM(E28,G28)</f>
         <v>140</v>
       </c>
-      <c r="L28" s="0" t="n">
+      <c r="J28" s="0" t="n">
+        <f aca="false">C28+G28</f>
+        <v>90</v>
+      </c>
+      <c r="O28" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>37</v>
@@ -1335,22 +1681,30 @@
         <v>298</v>
       </c>
       <c r="F29" s="0" t="n">
+        <f aca="false">E29-C29</f>
+        <v>261</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">SUM(E29:F29)</f>
+      <c r="H29" s="0" t="n">
+        <f aca="false">SUM(E29,G29)</f>
         <v>314</v>
       </c>
-      <c r="L29" s="0" t="n">
+      <c r="J29" s="0" t="n">
+        <f aca="false">C29+G29</f>
+        <v>53</v>
+      </c>
+      <c r="O29" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>35</v>
@@ -1362,22 +1716,30 @@
         <v>118</v>
       </c>
       <c r="F30" s="0" t="n">
+        <f aca="false">E30-C30</f>
+        <v>83</v>
+      </c>
+      <c r="G30" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">SUM(E30:F30)</f>
+      <c r="H30" s="0" t="n">
+        <f aca="false">SUM(E30,G30)</f>
         <v>133</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="J30" s="0" t="n">
+        <f aca="false">C30+G30</f>
+        <v>50</v>
+      </c>
+      <c r="O30" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>82</v>
@@ -1389,22 +1751,30 @@
         <v>300</v>
       </c>
       <c r="F31" s="0" t="n">
+        <f aca="false">E31-C31</f>
+        <v>218</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">SUM(E31:F31)</f>
+      <c r="H31" s="0" t="n">
+        <f aca="false">SUM(E31,G31)</f>
         <v>335</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="J31" s="0" t="n">
+        <f aca="false">C31+G31</f>
+        <v>117</v>
+      </c>
+      <c r="O31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>46</v>
@@ -1416,22 +1786,30 @@
         <v>296</v>
       </c>
       <c r="F32" s="0" t="n">
+        <f aca="false">E32-C32</f>
+        <v>250</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">SUM(E32:F32)</f>
+      <c r="H32" s="0" t="n">
+        <f aca="false">SUM(E32,G32)</f>
         <v>316</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="J32" s="0" t="n">
+        <f aca="false">C32+G32</f>
+        <v>66</v>
+      </c>
+      <c r="O32" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>79</v>
@@ -1443,22 +1821,30 @@
         <v>158</v>
       </c>
       <c r="F33" s="0" t="n">
+        <f aca="false">E33-C33</f>
+        <v>79</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <f aca="false">SUM(E33:F33)</f>
+      <c r="H33" s="0" t="n">
+        <f aca="false">SUM(E33,G33)</f>
         <v>193</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="J33" s="0" t="n">
+        <f aca="false">C33+G33</f>
+        <v>114</v>
+      </c>
+      <c r="O33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>58</v>
@@ -1470,22 +1856,30 @@
         <v>210</v>
       </c>
       <c r="F34" s="0" t="n">
+        <f aca="false">E34-C34</f>
+        <v>152</v>
+      </c>
+      <c r="G34" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <f aca="false">SUM(E34:F34)</f>
+      <c r="H34" s="0" t="n">
+        <f aca="false">SUM(E34,G34)</f>
         <v>236</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="J34" s="0" t="n">
+        <f aca="false">C34+G34</f>
+        <v>84</v>
+      </c>
+      <c r="O34" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>57</v>
@@ -1497,22 +1891,30 @@
         <v>292</v>
       </c>
       <c r="F35" s="0" t="n">
+        <f aca="false">E35-C35</f>
+        <v>235</v>
+      </c>
+      <c r="G35" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G35" s="0" t="n">
-        <f aca="false">SUM(E35:F35)</f>
+      <c r="H35" s="0" t="n">
+        <f aca="false">SUM(E35,G35)</f>
         <v>316</v>
       </c>
-      <c r="L35" s="0" t="n">
+      <c r="J35" s="0" t="n">
+        <f aca="false">C35+G35</f>
+        <v>81</v>
+      </c>
+      <c r="O35" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>117</v>
@@ -1524,22 +1926,30 @@
         <v>117</v>
       </c>
       <c r="F36" s="0" t="n">
+        <f aca="false">E36-C36</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G36" s="0" t="n">
-        <f aca="false">SUM(E36:F36)</f>
+      <c r="H36" s="0" t="n">
+        <f aca="false">SUM(E36,G36)</f>
         <v>167</v>
       </c>
-      <c r="L36" s="0" t="n">
+      <c r="J36" s="0" t="n">
+        <f aca="false">C36+G36</f>
+        <v>167</v>
+      </c>
+      <c r="O36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>82</v>
@@ -1551,22 +1961,30 @@
         <v>299</v>
       </c>
       <c r="F37" s="0" t="n">
+        <f aca="false">E37-C37</f>
+        <v>217</v>
+      </c>
+      <c r="G37" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <f aca="false">SUM(E37:F37)</f>
+      <c r="H37" s="0" t="n">
+        <f aca="false">SUM(E37,G37)</f>
         <v>334</v>
       </c>
-      <c r="L37" s="0" t="n">
+      <c r="J37" s="0" t="n">
+        <f aca="false">C37+G37</f>
+        <v>117</v>
+      </c>
+      <c r="O37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>129</v>
@@ -1578,22 +1996,30 @@
         <v>299</v>
       </c>
       <c r="F38" s="0" t="n">
+        <f aca="false">E38-C38</f>
+        <v>170</v>
+      </c>
+      <c r="G38" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="G38" s="0" t="n">
-        <f aca="false">SUM(E38:F38)</f>
+      <c r="H38" s="0" t="n">
+        <f aca="false">SUM(E38,G38)</f>
         <v>354</v>
       </c>
-      <c r="L38" s="0" t="n">
+      <c r="J38" s="0" t="n">
+        <f aca="false">C38+G38</f>
+        <v>184</v>
+      </c>
+      <c r="O38" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>41</v>
@@ -1605,22 +2031,30 @@
         <v>131</v>
       </c>
       <c r="F39" s="0" t="n">
+        <f aca="false">E39-C39</f>
+        <v>90</v>
+      </c>
+      <c r="G39" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <f aca="false">SUM(E39:F39)</f>
+      <c r="H39" s="0" t="n">
+        <f aca="false">SUM(E39,G39)</f>
         <v>149</v>
       </c>
-      <c r="L39" s="0" t="n">
+      <c r="J39" s="0" t="n">
+        <f aca="false">C39+G39</f>
+        <v>59</v>
+      </c>
+      <c r="O39" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>68</v>
@@ -1632,22 +2066,30 @@
         <v>299</v>
       </c>
       <c r="F40" s="0" t="n">
+        <f aca="false">E40-C40</f>
+        <v>231</v>
+      </c>
+      <c r="G40" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <f aca="false">SUM(E40:F40)</f>
+      <c r="H40" s="0" t="n">
+        <f aca="false">SUM(E40,G40)</f>
         <v>329</v>
       </c>
-      <c r="L40" s="0" t="n">
+      <c r="J40" s="0" t="n">
+        <f aca="false">C40+G40</f>
+        <v>98</v>
+      </c>
+      <c r="O40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C41" s="3" t="n">
         <v>36</v>
@@ -1659,22 +2101,30 @@
         <v>96</v>
       </c>
       <c r="F41" s="0" t="n">
+        <f aca="false">E41-C41</f>
+        <v>60</v>
+      </c>
+      <c r="G41" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <f aca="false">SUM(E41:F41)</f>
+      <c r="H41" s="0" t="n">
+        <f aca="false">SUM(E41,G41)</f>
         <v>112</v>
       </c>
-      <c r="L41" s="0" t="n">
+      <c r="J41" s="0" t="n">
+        <f aca="false">C41+G41</f>
+        <v>52</v>
+      </c>
+      <c r="O41" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>37</v>
@@ -1686,22 +2136,30 @@
         <v>136</v>
       </c>
       <c r="F42" s="0" t="n">
+        <f aca="false">E42-C42</f>
+        <v>99</v>
+      </c>
+      <c r="G42" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <f aca="false">SUM(E42:F42)</f>
+      <c r="H42" s="0" t="n">
+        <f aca="false">SUM(E42,G42)</f>
         <v>152</v>
       </c>
-      <c r="L42" s="0" t="n">
+      <c r="J42" s="0" t="n">
+        <f aca="false">C42+G42</f>
+        <v>53</v>
+      </c>
+      <c r="O42" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>44</v>
@@ -1713,22 +2171,30 @@
         <v>292</v>
       </c>
       <c r="F43" s="0" t="n">
+        <f aca="false">E43-C43</f>
+        <v>248</v>
+      </c>
+      <c r="G43" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="G43" s="0" t="n">
-        <f aca="false">SUM(E43:F43)</f>
+      <c r="H43" s="0" t="n">
+        <f aca="false">SUM(E43,G43)</f>
         <v>311</v>
       </c>
-      <c r="L43" s="0" t="n">
+      <c r="J43" s="0" t="n">
+        <f aca="false">C43+G43</f>
+        <v>63</v>
+      </c>
+      <c r="O43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>37</v>
@@ -1740,22 +2206,30 @@
         <v>296</v>
       </c>
       <c r="F44" s="0" t="n">
+        <f aca="false">E44-C44</f>
+        <v>259</v>
+      </c>
+      <c r="G44" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">SUM(E44:F44)</f>
+      <c r="H44" s="0" t="n">
+        <f aca="false">SUM(E44,G44)</f>
         <v>312</v>
       </c>
-      <c r="L44" s="0" t="n">
+      <c r="J44" s="0" t="n">
+        <f aca="false">C44+G44</f>
+        <v>53</v>
+      </c>
+      <c r="O44" s="0" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C45" s="3" t="n">
         <v>65</v>
@@ -1767,22 +2241,30 @@
         <v>163</v>
       </c>
       <c r="F45" s="0" t="n">
+        <f aca="false">E45-C45</f>
+        <v>98</v>
+      </c>
+      <c r="G45" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">SUM(E45:F45)</f>
+      <c r="H45" s="0" t="n">
+        <f aca="false">SUM(E45,G45)</f>
         <v>191</v>
       </c>
-      <c r="L45" s="0" t="n">
+      <c r="J45" s="0" t="n">
+        <f aca="false">C45+G45</f>
+        <v>93</v>
+      </c>
+      <c r="O45" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>40</v>
@@ -1794,22 +2276,30 @@
         <v>295</v>
       </c>
       <c r="F46" s="0" t="n">
+        <f aca="false">E46-C46</f>
+        <v>255</v>
+      </c>
+      <c r="G46" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G46" s="0" t="n">
-        <f aca="false">SUM(E46:F46)</f>
+      <c r="H46" s="0" t="n">
+        <f aca="false">SUM(E46,G46)</f>
         <v>312</v>
       </c>
-      <c r="L46" s="0" t="n">
+      <c r="J46" s="0" t="n">
+        <f aca="false">C46+G46</f>
+        <v>57</v>
+      </c>
+      <c r="O46" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>32</v>
@@ -1821,22 +2311,30 @@
         <v>292</v>
       </c>
       <c r="F47" s="0" t="n">
+        <f aca="false">E47-C47</f>
+        <v>260</v>
+      </c>
+      <c r="G47" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G47" s="0" t="n">
-        <f aca="false">SUM(E47:F47)</f>
+      <c r="H47" s="0" t="n">
+        <f aca="false">SUM(E47,G47)</f>
         <v>307</v>
       </c>
-      <c r="L47" s="0" t="n">
+      <c r="J47" s="0" t="n">
+        <f aca="false">C47+G47</f>
+        <v>47</v>
+      </c>
+      <c r="O47" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C48" s="3" t="n">
         <v>52</v>
@@ -1848,22 +2346,30 @@
         <v>134</v>
       </c>
       <c r="F48" s="0" t="n">
+        <f aca="false">E48-C48</f>
+        <v>82</v>
+      </c>
+      <c r="G48" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <f aca="false">SUM(E48:F48)</f>
+      <c r="H48" s="0" t="n">
+        <f aca="false">SUM(E48,G48)</f>
         <v>156</v>
       </c>
-      <c r="L48" s="0" t="n">
+      <c r="J48" s="0" t="n">
+        <f aca="false">C48+G48</f>
+        <v>74</v>
+      </c>
+      <c r="O48" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>67</v>
@@ -1875,22 +2381,30 @@
         <v>297</v>
       </c>
       <c r="F49" s="0" t="n">
+        <f aca="false">E49-C49</f>
+        <v>230</v>
+      </c>
+      <c r="G49" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <f aca="false">SUM(E49:F49)</f>
+      <c r="H49" s="0" t="n">
+        <f aca="false">SUM(E49,G49)</f>
         <v>326</v>
       </c>
-      <c r="L49" s="0" t="n">
+      <c r="J49" s="0" t="n">
+        <f aca="false">C49+G49</f>
+        <v>96</v>
+      </c>
+      <c r="O49" s="0" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>28</v>
@@ -1902,156 +2416,437 @@
         <v>128</v>
       </c>
       <c r="F50" s="0" t="n">
+        <f aca="false">E50-C50</f>
+        <v>100</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <f aca="false">SUM(E50:F50)</f>
+      <c r="H50" s="0" t="n">
+        <f aca="false">SUM(E50,G50)</f>
         <v>140</v>
       </c>
-      <c r="L50" s="0" t="n">
+      <c r="J50" s="0" t="n">
+        <f aca="false">C50+G50</f>
+        <v>40</v>
+      </c>
+      <c r="O50" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" s="0" t="n">
+      <c r="B51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="5" t="n">
         <f aca="false">SUM(C3:C50)</f>
         <v>3215</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="6" t="n">
         <f aca="false">SUM(D3:D50)</f>
         <v>29407</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="5" t="n">
         <f aca="false">SUM(E3:E50)</f>
         <v>10590</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="5" t="n">
         <f aca="false">SUM(F3:F50)</f>
+        <v>7375</v>
+      </c>
+      <c r="G51" s="7" t="n">
+        <f aca="false">SUM(G3:G50)</f>
         <v>1389</v>
       </c>
-      <c r="G51" s="0" t="n">
-        <f aca="false">SUM(G3:G50)</f>
+      <c r="H51" s="8" t="n">
+        <f aca="false">SUM(E51,G51)</f>
         <v>11979</v>
       </c>
-      <c r="I51" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J51" s="0" t="n">
-        <f aca="false">SUM(C51,F51)</f>
-        <v>4604</v>
+      <c r="I51" s="9" t="n">
+        <f aca="false">SUM(H3:H50)</f>
+        <v>11979</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L52" s="0" t="n">
-        <f aca="false">MIN(L3:L50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <f aca="false">MIN(C3:C50)</f>
-        <v>28</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <f aca="false">MIN(D3:D50)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <f aca="false">MIN(E3:E50)</f>
-        <v>94</v>
-      </c>
-      <c r="F53" s="1" t="n">
-        <f aca="false">MIN(F3:F50)</f>
-        <v>12</v>
-      </c>
-      <c r="G53" s="4" t="n">
-        <f aca="false">MIN(G3:G50)</f>
-        <v>111</v>
-      </c>
-      <c r="I53" s="0" t="s">
+      <c r="B52" s="10"/>
+      <c r="C52" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J53" s="0" t="n">
-        <f aca="false">J51/G51</f>
-        <v>0.384339260372318</v>
-      </c>
-    </row>
+      <c r="O52" s="0" t="n">
+        <f aca="false">MIN(O3:O50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="C54" s="1" t="n">
+        <f aca="false">MIN(C3:C50)</f>
+        <v>28</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <f aca="false">MIN(D3:D50)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">MIN(E3:E50)</f>
+        <v>94</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <f aca="false">MIN(F3:F50)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <f aca="false">MIN(G3:G50)</f>
+        <v>12</v>
+      </c>
+      <c r="H54" s="15" t="n">
+        <f aca="false">MIN(H3:H50)</f>
+        <v>111</v>
+      </c>
+      <c r="I54" s="15" t="n">
+        <f aca="false">MIN(I3:I50)</f>
+        <v>0</v>
+      </c>
+      <c r="J54" s="15" t="n">
+        <f aca="false">MIN(J3:J50)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <f aca="false">MAX(C3:C50)</f>
+        <v>157</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <f aca="false">MAX(D3:D50)</f>
+        <v>6875</v>
+      </c>
+      <c r="E55" s="1" t="n">
         <f aca="false">MAX(E3:E50)</f>
         <v>300</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="F55" s="1" t="n">
         <f aca="false">MAX(F3:F50)</f>
+        <v>261</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">MAX(G3:G50)</f>
         <v>67</v>
       </c>
-      <c r="G54" s="4" t="n">
-        <f aca="false">MAX(G3:G50)</f>
+      <c r="H55" s="15" t="n">
+        <f aca="false">MAX(H3:H50)</f>
         <v>359</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="0" t="n">
+      <c r="I55" s="15" t="n">
+        <f aca="false">MAX(I3:I50)</f>
+        <v>0</v>
+      </c>
+      <c r="J55" s="15" t="n">
+        <f aca="false">MAX(J3:J50)</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="0" t="n">
         <f aca="false">MEDIAN(C3:C50)</f>
         <v>54.5</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D57" s="0" t="n">
         <f aca="false">MEDIAN(D3:D50)</f>
         <v>203.5</v>
       </c>
-      <c r="E56" s="0" t="n">
+      <c r="E57" s="0" t="n">
         <f aca="false">MEDIAN(E3:E50)</f>
         <v>268</v>
       </c>
-      <c r="F56" s="0" t="n">
-        <f aca="false">MEDIAN(F3:F50)</f>
+      <c r="G57" s="0" t="n">
+        <f aca="false">MEDIAN(G3:G50)</f>
         <v>23</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <f aca="false">MEDIAN(G3:G50)</f>
+      <c r="H57" s="0" t="n">
+        <f aca="false">MEDIAN(H3:H50)</f>
         <v>289</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J58" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <f aca="false">SUM(C51,G51)</f>
+        <v>4604</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <f aca="false">K58/H51</f>
+        <v>0.384339260372318</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <f aca="false">ROUND(K59*1000,0)/10</f>
+        <v>38.4</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <f aca="false">ROUND(K60*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J61" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <f aca="false">F51</f>
+        <v>7375</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">ROUND(K61*1000,0)/10</f>
+        <v>737500</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J62" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <f aca="false">K61/H51</f>
+        <v>0.615660739627682</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <f aca="false">ROUND(K62*1000,0)/10</f>
+        <v>61.6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <f aca="false">SUM(K59,K62)</f>
+        <v>1</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <f aca="false">ROUND(K63*1000,0)/10</f>
+        <v>100</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <f aca="false">ROUND(K64*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L65" s="0" t="n">
+        <f aca="false">ROUND(K65*1000,0)/10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K66" s="7" t="n">
+        <f aca="false">G51/H51</f>
+        <v>0.11595291760581</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <f aca="false">ROUND(K66*1000,0)/10</f>
+        <v>11.6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K67" s="5" t="n">
+        <f aca="false">C51/H51</f>
+        <v>0.268386342766508</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <f aca="false">ROUND(K67*1000,0)/10</f>
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J68" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="K68" s="0" t="n">
+        <f aca="false">K66+K67</f>
+        <v>0.384339260372318</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <f aca="false">ROUND(K68*1000,0)/10</f>
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L69" s="0" t="n">
+        <f aca="false">ROUND(K69*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J70" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <f aca="false">F51/H51</f>
+        <v>0.615660739627682</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <f aca="false">ROUND(K70*1000,0)/10</f>
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L71" s="0" t="n">
+        <f aca="false">ROUND(K71*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="K72" s="0" t="n">
+        <f aca="false">K66+K67+K70</f>
+        <v>1</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <f aca="false">ROUND(K72*1000,0)/10</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L73" s="0" t="n">
+        <f aca="false">ROUND(K73*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L74" s="0" t="n">
+        <f aca="false">ROUND(K74*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J75" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <f aca="false">E51/H51</f>
+        <v>0.88404708239419</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <f aca="false">ROUND(K75*1000,0)/10</f>
+        <v>88.4</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J76" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="K76" s="0" t="n">
+        <f aca="false">K75+K66</f>
+        <v>1</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <f aca="false">ROUND(K76*1000,0)/10</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L77" s="0" t="n">
+        <f aca="false">ROUND(K77*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L78" s="0" t="n">
+        <f aca="false">ROUND(K78*1000,0)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J79" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K79" s="16" t="n">
+        <f aca="false">C51/E51</f>
+        <v>0.303588290840415</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <f aca="false">ROUND(K79*1000,0)/10</f>
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J80" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K80" s="16" t="n">
+        <f aca="false">F51/E51</f>
+        <v>0.696411709159584</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <f aca="false">ROUND(K80*1000,0)/10</f>
+        <v>69.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove multiple label and categories begore
</commit_message>
<xml_diff>
--- a/kaggle3/list_categories_dataset_draft.xlsx
+++ b/kaggle3/list_categories_dataset_draft.xlsx
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>10946</v>
+        <v>11089</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -660,16 +660,16 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
       <c r="F3">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="G3">
         <v>30</v>
@@ -706,7 +706,7 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>77</v>
@@ -715,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -732,7 +732,7 @@
         <v>51</v>
       </c>
       <c r="D6">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E6">
         <v>7</v>
@@ -752,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -761,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G7">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -775,16 +775,16 @@
         <v>19</v>
       </c>
       <c r="C8">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="G8">
         <v>22</v>
@@ -798,19 +798,19 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
       <c r="F9">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -844,7 +844,7 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>44</v>
@@ -853,10 +853,10 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -870,13 +870,13 @@
         <v>60</v>
       </c>
       <c r="D12">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G12">
         <v>26</v>
@@ -916,13 +916,13 @@
         <v>54</v>
       </c>
       <c r="D14">
-        <v>1378</v>
+        <v>1307</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="G14">
         <v>24</v>
@@ -939,7 +939,7 @@
         <v>53</v>
       </c>
       <c r="D15">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -985,13 +985,13 @@
         <v>256</v>
       </c>
       <c r="D17">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G17">
         <v>110</v>
@@ -1031,13 +1031,13 @@
         <v>130</v>
       </c>
       <c r="D19">
-        <v>1167</v>
+        <v>1149</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G19">
         <v>56</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G20">
         <v>56</v>
@@ -1077,7 +1077,7 @@
         <v>106</v>
       </c>
       <c r="D21">
-        <v>1666</v>
+        <v>1659</v>
       </c>
       <c r="E21">
         <v>13</v>
@@ -1100,13 +1100,13 @@
         <v>94</v>
       </c>
       <c r="D22">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G22">
         <v>41</v>
@@ -1169,13 +1169,13 @@
         <v>76</v>
       </c>
       <c r="D25">
-        <v>6564</v>
+        <v>6168</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F25">
-        <v>254</v>
+        <v>300</v>
       </c>
       <c r="G25">
         <v>33</v>
@@ -1189,19 +1189,19 @@
         <v>55</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26">
-        <v>2811</v>
+        <v>2379</v>
       </c>
       <c r="E26">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F26">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="G26">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1215,13 +1215,13 @@
         <v>61</v>
       </c>
       <c r="D27">
-        <v>1105</v>
+        <v>1055</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
       <c r="F27">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="G27">
         <v>26</v>
@@ -1261,13 +1261,13 @@
         <v>52</v>
       </c>
       <c r="D29">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G29">
         <v>23</v>
@@ -1284,13 +1284,13 @@
         <v>56</v>
       </c>
       <c r="D30">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="G30">
         <v>24</v>
@@ -1304,19 +1304,19 @@
         <v>65</v>
       </c>
       <c r="C31">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D31">
-        <v>1601</v>
+        <v>1516</v>
       </c>
       <c r="E31">
         <v>3</v>
       </c>
       <c r="F31">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="G31">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1330,13 +1330,13 @@
         <v>53</v>
       </c>
       <c r="D32">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G32">
         <v>23</v>
@@ -1353,13 +1353,13 @@
         <v>127</v>
       </c>
       <c r="D33">
-        <v>1126</v>
+        <v>1107</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G33">
         <v>54</v>
@@ -1396,7 +1396,7 @@
         <v>73</v>
       </c>
       <c r="C35">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35">
         <v>186</v>
@@ -1405,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G35">
         <v>28</v>
@@ -1422,13 +1422,13 @@
         <v>102</v>
       </c>
       <c r="D36">
-        <v>880</v>
+        <v>865</v>
       </c>
       <c r="E36">
         <v>13</v>
       </c>
       <c r="F36">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="G36">
         <v>44</v>
@@ -1445,13 +1445,13 @@
         <v>49</v>
       </c>
       <c r="D37">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E37">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F37">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="G37">
         <v>21</v>
@@ -1491,13 +1491,13 @@
         <v>67</v>
       </c>
       <c r="D39">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="E39">
         <v>7</v>
       </c>
       <c r="F39">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="G39">
         <v>29</v>
@@ -1511,19 +1511,19 @@
         <v>83</v>
       </c>
       <c r="C40">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E40">
         <v>4</v>
       </c>
       <c r="F40">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G40">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1537,13 +1537,13 @@
         <v>59</v>
       </c>
       <c r="D41">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E41">
         <v>2</v>
       </c>
       <c r="F41">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G41">
         <v>25</v>

</xml_diff>

<commit_message>
Send Chime n Finger snapping to dur split and update excel for last corrections. FSD11k final version
</commit_message>
<xml_diff>
--- a/kaggle3/list_categories_dataset_draft.xlsx
+++ b/kaggle3/list_categories_dataset_draft.xlsx
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>11074</v>
+        <v>11073</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -695,7 +695,7 @@
         <v>109</v>
       </c>
       <c r="G4">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1373,7 +1373,7 @@
         <v>71</v>
       </c>
       <c r="C34">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34">
         <v>49</v>
@@ -1382,10 +1382,10 @@
         <v>6</v>
       </c>
       <c r="F34">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G34">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1465,19 +1465,19 @@
         <v>79</v>
       </c>
       <c r="C38">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G38">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:7">

</xml_diff>